<commit_message>
(200206)Kkong_Solve 'out of bound' issue
PostProcessingShader의 루트 시그니쳐에 플레이어의 루트 파라미터를 정해주지 않았었음. 그래서 플레이어를 포스트 프로세싱 이전에 렌더함
</commit_message>
<xml_diff>
--- a/Client/ClientDoc/Errornote.xlsx
+++ b/Client/ClientDoc/Errornote.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraduationWork\Client\ClientDoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\졸작2\Client\ClientDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB83BC3-CCC0-4658-ABDD-38C154672513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C0EC4D-0897-4D90-97F5-438B12DA19B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4140" yWindow="-30" windowWidth="16605" windowHeight="15015" activeTab="1" xr2:uid="{230BCDDD-431A-4D7C-88B3-54A44AE19F74}"/>
+    <workbookView xWindow="-25320" yWindow="420" windowWidth="25440" windowHeight="15390" xr2:uid="{230BCDDD-431A-4D7C-88B3-54A44AE19F74}"/>
   </bookViews>
   <sheets>
     <sheet name="Error" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>발견 날짜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -93,6 +93,10 @@
   </si>
   <si>
     <t xml:space="preserve"> ID3D12CommandList::SetGraphicsRoot32BitConstants: RootParameterIndex [1] is out of bounds for the currently set root signature, which declares 1 root parameters.</t>
+  </si>
+  <si>
+    <t>PostProcessingShader의 루트 시그니쳐에 플레이어의 루트 파라미터를 정해주지 않았었음. 그래서 플레이어를 포스트 프로세싱 이전에 렌더함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -534,19 +538,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6010CCB8-5337-4488-8FF7-1A2F88F7C1B3}">
   <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
     <col min="5" max="5" width="92.5" customWidth="1"/>
-    <col min="6" max="6" width="86.375" customWidth="1"/>
+    <col min="6" max="6" width="86.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -563,7 +567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -580,20 +584,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>200207</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <v>200207</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -602,7 +610,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -611,7 +619,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -620,7 +628,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -629,7 +637,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -638,7 +646,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -647,7 +655,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -656,7 +664,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -665,7 +673,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -674,7 +682,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -683,7 +691,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -692,7 +700,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -701,7 +709,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -710,7 +718,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -719,7 +727,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -728,7 +736,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -737,7 +745,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -746,7 +754,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B22" s="1">
         <v>20</v>
       </c>
@@ -755,7 +763,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B23" s="1">
         <v>21</v>
       </c>
@@ -764,7 +772,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B24" s="1">
         <v>22</v>
       </c>
@@ -773,7 +781,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B25" s="1">
         <v>23</v>
       </c>
@@ -782,7 +790,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B26" s="1">
         <v>24</v>
       </c>
@@ -791,7 +799,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B27" s="1">
         <v>25</v>
       </c>
@@ -800,7 +808,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B28" s="1">
         <v>26</v>
       </c>
@@ -809,7 +817,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B29" s="1">
         <v>27</v>
       </c>
@@ -818,7 +826,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B30" s="1">
         <v>28</v>
       </c>
@@ -827,7 +835,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B31" s="1">
         <v>29</v>
       </c>
@@ -836,7 +844,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B32" s="1">
         <v>30</v>
       </c>
@@ -845,7 +853,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B33" s="1">
         <v>31</v>
       </c>
@@ -854,7 +862,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B34" s="1">
         <v>32</v>
       </c>
@@ -874,17 +882,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6003E8B3-757D-4013-803E-47761184C0B1}">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="60.25" customWidth="1"/>
-    <col min="5" max="5" width="95.625" customWidth="1"/>
+    <col min="4" max="4" width="60.19921875" customWidth="1"/>
+    <col min="5" max="5" width="95.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -892,7 +900,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="2:9" ht="99" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="104.4" x14ac:dyDescent="0.4">
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>8</v>
@@ -906,7 +914,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -921,7 +929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -929,7 +937,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -937,7 +945,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -945,7 +953,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -953,7 +961,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -961,7 +969,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -969,7 +977,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -977,7 +985,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -985,7 +993,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -993,7 +1001,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1001,7 +1009,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1009,7 +1017,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1017,7 +1025,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1025,7 +1033,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1033,7 +1041,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1041,7 +1049,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1049,7 +1057,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1057,7 +1065,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1065,7 +1073,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1073,7 +1081,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1081,7 +1089,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1089,7 +1097,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1097,7 +1105,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1105,7 +1113,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1113,7 +1121,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1121,7 +1129,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1129,7 +1137,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1137,7 +1145,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>

</xml_diff>

<commit_message>
Revert "Revert "(200225)Ahna_SkyBox complete""
This reverts commit a3e882a043e8a17982a6488aee0fec94611d9744.
</commit_message>
<xml_diff>
--- a/Client/ClientDoc/Errornote.xlsx
+++ b/Client/ClientDoc/Errornote.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraduationWork\Client\ClientDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558C3C3E-714A-4244-877A-7CDF9282C18E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA91DFF7-AEC4-443F-A3B0-672007686866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4725" yWindow="705" windowWidth="21600" windowHeight="11385" xr2:uid="{230BCDDD-431A-4D7C-88B3-54A44AE19F74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>발견 날짜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,6 +136,14 @@
 D3D12 WARNING: Live           ID3D12DescriptorHeap :      4 [ STATE_CREATION WARNING #255: LIVE_OBJECT_SUMMARY]
 D3D12 WARNING: Live                 IDXGISwapChain :      1 [ STATE_CREATION WARNING #255: LIVE_OBJECT_SUMMARY]
 D3D12 WARNING: Live          ID3D12LifetimeTracker :      1 [ STATE_CREATION WARNING #255: LIVE_OBJECT_SUMMARY]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D3D12 ERROR: ID3D12CommandList::DrawInstanced: No pipeline state has been set in this command list.  The runtime will use a default no-op pipeline state. [ EXECUTION ERROR #1045: COMMAND_LIST_PIPELINE_STATE_NOT_SET]</t>
+  </si>
+  <si>
+    <t>createshader가 잘 오버로드 되지않았고 파이프라인스테이트상태를 new로 생성해주지 않았다. 파이프라인을 생성해주자.	 m_nPipelineStates = 1;
+	 m_ppd3dPipelineStates = new ID3D12PipelineState * [m_nPipelineStates];</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -575,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6010CCB8-5337-4488-8FF7-1A2F88F7C1B3}">
   <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -707,14 +715,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="1">

</xml_diff>